<commit_message>
Added linear flutter results
</commit_message>
<xml_diff>
--- a/01_2022_SciTech_Riso_Cesnik/08_Linear_Flutter/stability.xlsx
+++ b/01_2022_SciTech_Riso_Cesnik/08_Linear_Flutter/stability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOSITORIES\AePW3-LDWG\01_2022_SciTech_Riso_Cesnik\08_Linear_Flutter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criso3\Repositories\09_Data\AePW3-LDWG\01_2022_SciTech_Riso_Cesnik\08_Linear_Flutter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA39F886-9F40-4217-B57F-F1F0A651C7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F5EA3D-CE80-435A-87A3-AD7F51FBBCF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="648" windowWidth="12924" windowHeight="11604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="650" windowWidth="12920" windowHeight="11600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flutter and divergence" sheetId="1" r:id="rId1"/>
@@ -125,14 +125,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,344 +421,344 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>74.773899999999998</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>75.700999999999993</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <f>(D3-C3)/C3*100</f>
         <v>1.2398711315044366</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>16.5871</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>16.153700000000001</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <f t="shared" ref="E4:E5" si="0">(D4-C4)/C4*100</f>
         <v>-2.6128738598067107</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>85.497500000000002</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>83.600899999999996</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <f t="shared" si="0"/>
         <v>-2.218310476914537</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>82.9041</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>83.601399999999998</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <f>(D9-C9)/C9*100</f>
         <v>0.84109229820961628</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>18.170300000000001</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>17.724699999999999</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <f t="shared" ref="E10:E11" si="1">(D10-C10)/C10*100</f>
         <v>-2.4523535659840645</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>85.494699999999995</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>83.616799999999998</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <f t="shared" si="1"/>
         <v>-2.1965104269621354</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>86.525000000000006</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>91.7714</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <f>(D15-C15)/C15*100</f>
         <v>6.0634498699797676</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>16.159099999999999</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>12.8041128719477</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <f>(D16-C16)/C16*100</f>
         <v>-20.762215272213794</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>100.9688</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>98.314800000000005</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <f>(D17-C17)/C17*100</f>
         <v>-2.6285347552907399</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <v>67.300899999999999</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>72.403700000000001</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="4">
         <f>(D21-C21)/C21*100</f>
         <v>7.5820679961189255</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <v>34.722499999999997</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="4">
         <v>34.721699999999998</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="4">
         <f t="shared" ref="E22:E23" si="2">(D22-C22)/C22*100</f>
         <v>-2.3039815681420855E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <v>100.9657</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="4">
         <v>98.315399999999997</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="4">
         <f t="shared" si="2"/>
         <v>-2.6249508496449798</v>
       </c>

</xml_diff>